<commit_message>
uploading final model and clearing the sheets
</commit_message>
<xml_diff>
--- a/Scoring Sheet Training Files.xlsx
+++ b/Scoring Sheet Training Files.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="48">
   <si>
     <t>Team Number:</t>
   </si>
@@ -172,7 +172,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.000%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -339,7 +339,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5258,7 +5258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AY57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -6022,7 +6022,7 @@
         <v>2.4710245215361932</v>
       </c>
       <c r="AY15" s="16">
-        <f>(AW3-AW15)/AW3</f>
+        <f>($AW$3-AW15)/$AW$3</f>
         <v>0.11511508941479109</v>
       </c>
     </row>
@@ -6042,7 +6042,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" ref="F15:P22" si="19">1/24</f>
+        <f t="shared" ref="F16:P22" si="19">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G16" s="4">
@@ -6146,8 +6146,68 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:34" ht="18.75">
+      <c r="AJ16">
+        <f t="shared" ref="AJ16:AJ22" si="22">D16*LOG((1/D16),2)</f>
+        <v>0.5</v>
+      </c>
+      <c r="AK16">
+        <f t="shared" ref="AK16:AK22" si="23">E16*LOG((1/E16),2)</f>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AL16">
+        <f t="shared" ref="AL16:AL22" si="24">F16*LOG((1/F16),2)</f>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AM16">
+        <f t="shared" ref="AM16:AM22" si="25">G16*LOG((1/G16),2)</f>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AN16">
+        <f t="shared" ref="AN16:AN22" si="26">H16*LOG((1/H16),2)</f>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AO16">
+        <f t="shared" ref="AO16:AO22" si="27">I16*LOG((1/I16),2)</f>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AP16">
+        <f t="shared" ref="AP16:AP22" si="28">J16*LOG((1/J16),2)</f>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AQ16">
+        <f t="shared" ref="AQ16:AQ22" si="29">K16*LOG((1/K16),2)</f>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AR16">
+        <f t="shared" ref="AR16:AR22" si="30">L16*LOG((1/L16),2)</f>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AS16">
+        <f t="shared" ref="AS16:AS22" si="31">M16*LOG((1/M16),2)</f>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AT16">
+        <f t="shared" ref="AT16:AT22" si="32">N16*LOG((1/N16),2)</f>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AU16">
+        <f t="shared" ref="AU16:AU22" si="33">O16*LOG((1/O16),2)</f>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AV16">
+        <f t="shared" ref="AV16:AV22" si="34">P16*LOG((1/P16),2)</f>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AW16">
+        <f t="shared" ref="AW16:AW22" si="35">SUM(AJ16:AV16)</f>
+        <v>2.7924812503605789</v>
+      </c>
+      <c r="AY16" s="16">
+        <f t="shared" ref="AY16:AY22" si="36">($AW$3-AW16)/$AW$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:51" ht="18.75">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -6267,8 +6327,68 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:34" ht="18.75">
+      <c r="AJ17">
+        <f t="shared" si="22"/>
+        <v>0.5</v>
+      </c>
+      <c r="AK17">
+        <f t="shared" si="23"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AL17">
+        <f t="shared" si="24"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AM17">
+        <f t="shared" si="25"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AN17">
+        <f t="shared" si="26"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AO17">
+        <f t="shared" si="27"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AP17">
+        <f t="shared" si="28"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AQ17">
+        <f t="shared" si="29"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AR17">
+        <f t="shared" si="30"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AS17">
+        <f t="shared" si="31"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AT17">
+        <f t="shared" si="32"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AU17">
+        <f t="shared" si="33"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AV17">
+        <f t="shared" si="34"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AW17">
+        <f t="shared" si="35"/>
+        <v>2.7924812503605789</v>
+      </c>
+      <c r="AY17" s="16">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:51" ht="18.75">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -6388,8 +6508,68 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:34" ht="18.75">
+      <c r="AJ18">
+        <f t="shared" si="22"/>
+        <v>0.5</v>
+      </c>
+      <c r="AK18">
+        <f t="shared" si="23"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AL18">
+        <f t="shared" si="24"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AM18">
+        <f t="shared" si="25"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AN18">
+        <f t="shared" si="26"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AO18">
+        <f t="shared" si="27"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AP18">
+        <f t="shared" si="28"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AQ18">
+        <f t="shared" si="29"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AR18">
+        <f t="shared" si="30"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AS18">
+        <f t="shared" si="31"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AT18">
+        <f t="shared" si="32"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AU18">
+        <f t="shared" si="33"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AV18">
+        <f t="shared" si="34"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AW18">
+        <f t="shared" si="35"/>
+        <v>2.7924812503605789</v>
+      </c>
+      <c r="AY18" s="16">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:51" ht="18.75">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -6509,8 +6689,68 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:34" ht="18.75">
+      <c r="AJ19">
+        <f t="shared" si="22"/>
+        <v>0.5</v>
+      </c>
+      <c r="AK19">
+        <f t="shared" si="23"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AL19">
+        <f t="shared" si="24"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AM19">
+        <f t="shared" si="25"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AN19">
+        <f t="shared" si="26"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AO19">
+        <f t="shared" si="27"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AP19">
+        <f t="shared" si="28"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AQ19">
+        <f t="shared" si="29"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AR19">
+        <f t="shared" si="30"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AS19">
+        <f t="shared" si="31"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AT19">
+        <f t="shared" si="32"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AU19">
+        <f t="shared" si="33"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AV19">
+        <f t="shared" si="34"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AW19">
+        <f t="shared" si="35"/>
+        <v>2.7924812503605789</v>
+      </c>
+      <c r="AY19" s="16">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:51" ht="18.75">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -6630,8 +6870,68 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:34" ht="18.75">
+      <c r="AJ20">
+        <f t="shared" si="22"/>
+        <v>0.5</v>
+      </c>
+      <c r="AK20">
+        <f t="shared" si="23"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AL20">
+        <f t="shared" si="24"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AM20">
+        <f t="shared" si="25"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AN20">
+        <f t="shared" si="26"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AO20">
+        <f t="shared" si="27"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AP20">
+        <f t="shared" si="28"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AQ20">
+        <f t="shared" si="29"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AR20">
+        <f t="shared" si="30"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AS20">
+        <f t="shared" si="31"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AT20">
+        <f t="shared" si="32"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AU20">
+        <f t="shared" si="33"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AV20">
+        <f t="shared" si="34"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AW20">
+        <f t="shared" si="35"/>
+        <v>2.7924812503605789</v>
+      </c>
+      <c r="AY20" s="16">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:51" ht="18.75">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -6751,8 +7051,68 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:34" ht="18.75">
+      <c r="AJ21">
+        <f t="shared" si="22"/>
+        <v>0.5</v>
+      </c>
+      <c r="AK21">
+        <f t="shared" si="23"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AL21">
+        <f t="shared" si="24"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AM21">
+        <f t="shared" si="25"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AN21">
+        <f t="shared" si="26"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AO21">
+        <f t="shared" si="27"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AP21">
+        <f t="shared" si="28"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AQ21">
+        <f t="shared" si="29"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AR21">
+        <f t="shared" si="30"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AS21">
+        <f t="shared" si="31"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AT21">
+        <f t="shared" si="32"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AU21">
+        <f t="shared" si="33"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AV21">
+        <f t="shared" si="34"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AW21">
+        <f t="shared" si="35"/>
+        <v>2.7924812503605789</v>
+      </c>
+      <c r="AY21" s="16">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:51" ht="18.75">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -6872,8 +7232,68 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:34">
+      <c r="AJ22">
+        <f t="shared" si="22"/>
+        <v>0.5</v>
+      </c>
+      <c r="AK22">
+        <f t="shared" si="23"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AL22">
+        <f t="shared" si="24"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AM22">
+        <f t="shared" si="25"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AN22">
+        <f t="shared" si="26"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AO22">
+        <f t="shared" si="27"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AP22">
+        <f t="shared" si="28"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AQ22">
+        <f t="shared" si="29"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AR22">
+        <f t="shared" si="30"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AS22">
+        <f t="shared" si="31"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AT22">
+        <f t="shared" si="32"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AU22">
+        <f t="shared" si="33"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AV22">
+        <f t="shared" si="34"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AW22">
+        <f t="shared" si="35"/>
+        <v>2.7924812503605789</v>
+      </c>
+      <c r="AY22" s="16">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:51">
       <c r="D23" s="5" t="s">
         <v>34</v>
       </c>
@@ -6882,7 +7302,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="18.75">
+    <row r="24" spans="1:51" ht="18.75">
       <c r="D24" s="1">
         <v>0</v>
       </c>
@@ -6931,7 +7351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:34">
+    <row r="25" spans="1:51">
       <c r="A25" s="15" t="s">
         <v>44</v>
       </c>
@@ -6939,7 +7359,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="18.75">
+    <row r="26" spans="1:51" ht="18.75">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -6953,51 +7373,51 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F26" s="3">
-        <f t="shared" ref="F26:P33" si="22">1/24</f>
+        <f t="shared" ref="F26:P33" si="37">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G26" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I26" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J26" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K26" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L26" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M26" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N26" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O26" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P26" s="3">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R26" s="3">
-        <f t="shared" ref="R26:R33" si="23">SUM(D26:P26)</f>
+        <f t="shared" ref="R26:R33" si="38">SUM(D26:P26)</f>
         <v>0.99999999999999956</v>
       </c>
       <c r="T26" s="11">
@@ -7010,55 +7430,55 @@
         <v>0</v>
       </c>
       <c r="W26">
-        <f t="shared" ref="W26:AH33" si="24">LOG(E26/E$3, 2)*E$35</f>
+        <f t="shared" ref="W26:AH33" si="39">LOG(E26/E$3, 2)*E$35</f>
         <v>0</v>
       </c>
       <c r="X26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Z26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AB26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AC26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AD26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AE26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AF26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AG26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AH26">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:34" ht="18.75">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:51" ht="18.75">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -7072,112 +7492,112 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F27" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J27" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L27" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M27" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N27" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O27" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P27" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R27" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="38"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T27" s="11">
-        <f t="shared" ref="T27:T33" si="25">SUM(V27:AH27)</f>
+        <f t="shared" ref="T27:T33" si="40">SUM(V27:AH27)</f>
         <v>0</v>
       </c>
       <c r="U27" s="13"/>
       <c r="V27">
-        <f t="shared" ref="V27:V33" si="26">LOG(D27/D$3, 2)*D$35</f>
+        <f t="shared" ref="V27:V33" si="41">LOG(D27/D$3, 2)*D$35</f>
         <v>0</v>
       </c>
       <c r="W27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Z27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AB27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AC27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AD27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AE27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AF27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AG27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AH27">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:34" ht="18.75">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:51" ht="18.75">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -7187,116 +7607,116 @@
         <v>0.5</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" ref="E28:E33" si="27">1/24</f>
+        <f t="shared" ref="E28:E33" si="42">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F28" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G28" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J28" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K28" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L28" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M28" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N28" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O28" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P28" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R28" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="38"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T28" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="U28" s="13"/>
       <c r="V28">
-        <f t="shared" si="26"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="W28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Z28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AB28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AC28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AD28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AE28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AF28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AG28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AH28">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:34" ht="18.75">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:51" ht="18.75">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -7306,116 +7726,116 @@
         <v>0.5</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="42"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P29" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R29" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="38"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T29" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="U29" s="13"/>
       <c r="V29">
-        <f t="shared" si="26"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="W29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Z29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AB29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AC29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AD29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AE29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AF29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AG29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AH29">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:34" ht="18.75">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:51" ht="18.75">
       <c r="A30" t="s">
         <v>6</v>
       </c>
@@ -7425,116 +7845,116 @@
         <v>0.5</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="42"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F30" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J30" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K30" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L30" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M30" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N30" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O30" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P30" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R30" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="38"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T30" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="U30" s="13"/>
       <c r="V30">
-        <f t="shared" si="26"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="W30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Z30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AB30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AC30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AD30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AE30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AF30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AG30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AH30">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:34" ht="18.75">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:51" ht="18.75">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -7544,116 +7964,116 @@
         <v>0.5</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="42"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F31" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J31" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K31" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L31" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M31" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N31" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O31" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P31" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R31" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="38"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T31" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="U31" s="13"/>
       <c r="V31">
-        <f t="shared" si="26"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="W31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AB31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AC31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AD31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AE31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AF31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AG31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AH31">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:34" ht="18.75">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:51" ht="18.75">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -7663,112 +8083,112 @@
         <v>0.5</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="42"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F32" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J32" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K32" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L32" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M32" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N32" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O32" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P32" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R32" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="38"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T32" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="U32" s="13"/>
       <c r="V32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="W32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AB32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AC32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AD32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AE32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AF32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AG32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AH32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
     </row>
@@ -7782,47 +8202,47 @@
         <v>0.5</v>
       </c>
       <c r="E33" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="42"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F33" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G33" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J33" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K33" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L33" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M33" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N33" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O33" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="37"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P33" s="4">
@@ -7830,60 +8250,60 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R33" s="3">
-        <f t="shared" si="23"/>
+        <f t="shared" si="38"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T33" s="11">
-        <f t="shared" si="25"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="U33" s="13"/>
       <c r="V33">
-        <f t="shared" si="26"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="W33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="X33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Z33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AA33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AB33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AC33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AD33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AE33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AF33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AG33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="AH33">
@@ -7982,51 +8402,51 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F37" s="4">
-        <f t="shared" ref="F37:P44" si="28">1/24</f>
+        <f t="shared" ref="F37:P44" si="43">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G37" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H37" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I37" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J37" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K37" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L37" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M37" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N37" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O37" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P37" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R37" s="3">
-        <f t="shared" ref="R37:R44" si="29">SUM(D37:P37)</f>
+        <f t="shared" ref="R37:R44" si="44">SUM(D37:P37)</f>
         <v>0.99999999999999956</v>
       </c>
       <c r="T37" s="11">
@@ -8039,51 +8459,51 @@
         <v>0</v>
       </c>
       <c r="W37">
-        <f t="shared" ref="W37:AH44" si="30">LOG(E37/E$3, 2)*E$46</f>
+        <f t="shared" ref="W37:AH44" si="45">LOG(E37/E$3, 2)*E$46</f>
         <v>0</v>
       </c>
       <c r="X37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Y37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Z37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AA37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AB37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AC37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AD37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AE37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AF37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AG37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AH37">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
     </row>
@@ -8097,112 +8517,112 @@
         <v>0.5</v>
       </c>
       <c r="E38" s="4">
-        <f t="shared" ref="E38:E44" si="31">1/24</f>
+        <f t="shared" ref="E38:E44" si="46">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F38" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G38" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I38" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J38" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K38" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L38" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M38" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N38" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O38" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P38" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R38" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="44"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T38" s="11">
-        <f t="shared" ref="T38:T44" si="32">SUM(V38:AH38)</f>
+        <f t="shared" ref="T38:T44" si="47">SUM(V38:AH38)</f>
         <v>0</v>
       </c>
       <c r="U38" s="13"/>
       <c r="V38">
-        <f t="shared" ref="V38:V44" si="33">LOG(D38/D$3, 2)*D$46</f>
+        <f t="shared" ref="V38:V44" si="48">LOG(D38/D$3, 2)*D$46</f>
         <v>0</v>
       </c>
       <c r="W38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="X38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Y38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Z38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AA38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AB38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AC38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AD38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AE38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AF38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AG38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AH38">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
     </row>
@@ -8216,112 +8636,112 @@
         <v>0.5</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P39" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R39" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="44"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T39" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="U39" s="13"/>
       <c r="V39">
-        <f t="shared" si="33"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="X39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Y39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Z39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AA39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AB39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AC39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AD39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AE39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AF39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AG39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AH39">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
     </row>
@@ -8335,112 +8755,112 @@
         <v>0.5</v>
       </c>
       <c r="E40" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F40" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G40" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H40" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I40" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J40" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K40" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L40" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M40" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N40" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O40" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P40" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R40" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="44"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T40" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="U40" s="13"/>
       <c r="V40">
-        <f t="shared" si="33"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="X40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Y40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Z40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AA40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AB40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AC40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AD40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AE40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AF40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AG40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AH40">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
     </row>
@@ -8454,112 +8874,112 @@
         <v>0.5</v>
       </c>
       <c r="E41" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F41" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G41" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H41" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I41" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J41" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K41" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L41" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M41" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N41" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O41" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P41" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R41" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="44"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T41" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="U41" s="13"/>
       <c r="V41">
-        <f t="shared" si="33"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="X41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Y41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Z41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AA41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AB41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AC41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AD41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AE41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AF41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AG41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AH41">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
     </row>
@@ -8573,112 +8993,112 @@
         <v>0.5</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F42" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G42" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H42" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I42" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J42" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K42" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L42" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M42" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N42" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O42" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P42" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R42" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="44"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T42" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="U42" s="13"/>
       <c r="V42">
-        <f t="shared" si="33"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="X42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Y42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Z42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AA42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AB42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AC42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AD42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AE42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AF42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AG42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AH42">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
     </row>
@@ -8692,112 +9112,112 @@
         <v>0.5</v>
       </c>
       <c r="E43" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F43" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G43" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H43" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I43" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J43" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K43" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L43" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M43" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N43" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O43" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P43" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R43" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="44"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T43" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="U43" s="13"/>
       <c r="V43">
-        <f t="shared" si="33"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="X43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Y43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Z43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AA43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AB43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AC43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AD43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AE43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AF43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AG43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AH43">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
     </row>
@@ -8811,108 +9231,108 @@
         <v>0.5</v>
       </c>
       <c r="E44" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="46"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F44" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G44" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H44" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I44" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J44" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K44" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L44" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M44" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N44" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O44" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P44" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="43"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R44" s="3">
-        <f t="shared" si="29"/>
+        <f t="shared" si="44"/>
         <v>0.99999999999999956</v>
       </c>
       <c r="T44" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="U44" s="13"/>
       <c r="V44">
-        <f t="shared" si="33"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="W44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="X44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Y44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Z44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AA44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AB44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AC44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AD44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AE44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AF44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AG44">
-        <f t="shared" si="30"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="AH44">
@@ -8978,1021 +9398,187 @@
       </c>
     </row>
     <row r="47" spans="1:34">
-      <c r="A47" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" t="s">
-        <v>13</v>
-      </c>
+      <c r="A47" s="15"/>
     </row>
     <row r="48" spans="1:34" ht="18.75">
-      <c r="A48" t="s">
-        <v>2</v>
-      </c>
       <c r="B48" s="1"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E48" s="4">
-        <f>1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F48" s="4">
-        <f t="shared" ref="F48:P55" si="34">1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G48" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H48" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I48" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J48" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K48" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L48" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M48" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="N48" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="O48" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="P48" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="R48" s="3">
-        <f t="shared" ref="R48:R55" si="35">SUM(D48:P48)</f>
-        <v>0.99999999999999956</v>
-      </c>
-      <c r="T48" s="11">
-        <f>SUM(V48:AH48)</f>
-        <v>0</v>
-      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="R48" s="3"/>
+      <c r="T48" s="11"/>
       <c r="U48" s="13"/>
-      <c r="V48">
-        <f>LOG(D48/D$3, 2)*D$57</f>
-        <v>0</v>
-      </c>
-      <c r="W48">
-        <f t="shared" ref="W48:AH55" si="36">LOG(E48/E$3, 2)*E$57</f>
-        <v>0</v>
-      </c>
-      <c r="X48">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Y48">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Z48">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AA48">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AB48">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AC48">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AD48">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AE48">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AF48">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AG48">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AH48">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:34" ht="18.75">
-      <c r="A49" t="s">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="49" spans="2:21" ht="18.75">
       <c r="B49" s="1"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E49" s="4">
-        <f t="shared" ref="E49:E55" si="37">1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F49" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G49" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H49" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I49" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J49" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K49" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L49" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M49" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="N49" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="O49" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="P49" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="R49" s="3">
-        <f t="shared" si="35"/>
-        <v>0.99999999999999956</v>
-      </c>
-      <c r="T49" s="11">
-        <f t="shared" ref="T49:T55" si="38">SUM(V49:AH49)</f>
-        <v>0</v>
-      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+      <c r="R49" s="3"/>
+      <c r="T49" s="11"/>
       <c r="U49" s="13"/>
-      <c r="V49">
-        <f t="shared" ref="V49:V55" si="39">LOG(D49/D$3, 2)*D$57</f>
-        <v>0</v>
-      </c>
-      <c r="W49">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="X49">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Y49">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Z49">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AA49">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AB49">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AC49">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AD49">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AE49">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AF49">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AG49">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AH49">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:34" ht="18.75">
-      <c r="A50" t="s">
-        <v>4</v>
-      </c>
+    </row>
+    <row r="50" spans="2:21" ht="18.75">
       <c r="B50" s="1"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E50" s="4">
-        <f t="shared" si="37"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F50" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G50" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H50" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I50" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J50" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K50" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L50" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M50" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="N50" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="O50" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="P50" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="R50" s="3">
-        <f t="shared" si="35"/>
-        <v>0.99999999999999956</v>
-      </c>
-      <c r="T50" s="11">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="R50" s="3"/>
+      <c r="T50" s="11"/>
       <c r="U50" s="13"/>
-      <c r="V50">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="W50">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="X50">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Y50">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Z50">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AA50">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AB50">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AC50">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AD50">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AE50">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AF50">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AG50">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AH50">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:34" ht="18.75">
-      <c r="A51" t="s">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="51" spans="2:21" ht="18.75">
       <c r="B51" s="1"/>
       <c r="C51" s="2"/>
-      <c r="D51" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E51" s="4">
-        <f t="shared" si="37"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F51" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G51" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H51" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I51" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J51" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K51" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L51" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M51" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="N51" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="O51" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="P51" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="R51" s="3">
-        <f t="shared" si="35"/>
-        <v>0.99999999999999956</v>
-      </c>
-      <c r="T51" s="11">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="R51" s="3"/>
+      <c r="T51" s="11"/>
       <c r="U51" s="13"/>
-      <c r="V51">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="W51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="X51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Y51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Z51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AA51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AB51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AC51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AD51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AE51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AF51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AG51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AH51">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:34" ht="18.75">
-      <c r="A52" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="52" spans="2:21" ht="18.75">
       <c r="B52" s="1"/>
       <c r="C52" s="2"/>
-      <c r="D52" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E52" s="4">
-        <f t="shared" si="37"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F52" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G52" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H52" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I52" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J52" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K52" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L52" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M52" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="N52" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="O52" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="P52" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="R52" s="3">
-        <f t="shared" si="35"/>
-        <v>0.99999999999999956</v>
-      </c>
-      <c r="T52" s="11">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4"/>
+      <c r="R52" s="3"/>
+      <c r="T52" s="11"/>
       <c r="U52" s="13"/>
-      <c r="V52">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="W52">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="X52">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Y52">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Z52">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AA52">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AB52">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AC52">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AD52">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AE52">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AF52">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AG52">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AH52">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:34" ht="18.75">
-      <c r="A53" t="s">
-        <v>7</v>
-      </c>
+    </row>
+    <row r="53" spans="2:21" ht="18.75">
       <c r="B53" s="1"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E53" s="4">
-        <f t="shared" si="37"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F53" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G53" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H53" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I53" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J53" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K53" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L53" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M53" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="N53" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="O53" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="P53" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="R53" s="3">
-        <f t="shared" si="35"/>
-        <v>0.99999999999999956</v>
-      </c>
-      <c r="T53" s="11">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4"/>
+      <c r="R53" s="3"/>
+      <c r="T53" s="11"/>
       <c r="U53" s="13"/>
-      <c r="V53">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="W53">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="X53">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Y53">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Z53">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AA53">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AB53">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AC53">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AD53">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AE53">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AF53">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AG53">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AH53">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:34" ht="18.75">
-      <c r="A54" t="s">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="54" spans="2:21" ht="18.75">
       <c r="B54" s="1"/>
       <c r="C54" s="2"/>
-      <c r="D54" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E54" s="4">
-        <f t="shared" si="37"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F54" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G54" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H54" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I54" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J54" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K54" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L54" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M54" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="N54" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="O54" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="P54" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="R54" s="3">
-        <f t="shared" si="35"/>
-        <v>0.99999999999999956</v>
-      </c>
-      <c r="T54" s="11">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="R54" s="3"/>
+      <c r="T54" s="11"/>
       <c r="U54" s="13"/>
-      <c r="V54">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="W54">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="X54">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Y54">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Z54">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AA54">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AB54">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AC54">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AD54">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AE54">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AF54">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AG54">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AH54">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:34" ht="18.75">
-      <c r="A55" t="s">
-        <v>9</v>
-      </c>
+    </row>
+    <row r="55" spans="2:21" ht="18.75">
       <c r="B55" s="1"/>
       <c r="C55" s="2"/>
-      <c r="D55" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E55" s="4">
-        <f t="shared" si="37"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="F55" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="G55" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="H55" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="I55" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="J55" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="K55" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="L55" s="4">
-        <f>1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="M55" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="N55" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="O55" s="4">
-        <f t="shared" si="34"/>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="P55" s="4">
-        <f>1/24</f>
-        <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="R55" s="3">
-        <f t="shared" si="35"/>
-        <v>0.99999999999999956</v>
-      </c>
-      <c r="T55" s="11">
-        <f t="shared" si="38"/>
-        <v>0</v>
-      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4"/>
+      <c r="R55" s="3"/>
+      <c r="T55" s="11"/>
       <c r="U55" s="13"/>
-      <c r="V55">
-        <f t="shared" si="39"/>
-        <v>0</v>
-      </c>
-      <c r="W55">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="X55">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Y55">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="Z55">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AA55">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AB55">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AC55">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AD55">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AE55">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AF55">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AG55">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-      <c r="AH55">
-        <f t="shared" si="36"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:34">
-      <c r="D56" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="T56" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="57" spans="1:34" ht="18.75">
-      <c r="D57" s="1">
-        <v>0</v>
-      </c>
-      <c r="E57" s="1">
-        <v>0</v>
-      </c>
-      <c r="F57" s="1">
-        <v>0</v>
-      </c>
-      <c r="G57" s="1">
-        <v>0</v>
-      </c>
-      <c r="H57" s="1">
-        <v>0</v>
-      </c>
-      <c r="I57" s="1">
-        <v>0</v>
-      </c>
-      <c r="J57" s="1">
-        <v>0</v>
-      </c>
-      <c r="K57" s="1">
-        <v>0</v>
-      </c>
-      <c r="L57" s="1">
-        <v>0</v>
-      </c>
-      <c r="M57" s="1">
-        <v>0</v>
-      </c>
-      <c r="N57" s="1">
-        <v>0</v>
-      </c>
-      <c r="O57" s="1">
-        <v>0</v>
-      </c>
-      <c r="P57" s="1">
-        <v>1</v>
-      </c>
-      <c r="R57" s="3">
-        <f>SUM(D57:P57)</f>
-        <v>1</v>
-      </c>
-      <c r="T57" s="14">
-        <f>AVERAGE(T48:T55)</f>
-        <v>0</v>
-      </c>
+    </row>
+    <row r="56" spans="2:21">
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" spans="2:21" ht="18.75">
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="R57" s="3"/>
+      <c r="T57" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
miscellaneous training file uploads
</commit_message>
<xml_diff>
--- a/Scoring Sheet Training Files.xlsx
+++ b/Scoring Sheet Training Files.xlsx
@@ -5258,9 +5258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AY57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
@@ -5910,12 +5908,12 @@
       </c>
       <c r="T15" s="11">
         <f>SUM(V15:AH15)</f>
-        <v>0</v>
+        <v>0.2240402742179301</v>
       </c>
       <c r="U15" s="13"/>
       <c r="V15">
         <f t="shared" ref="V15:AH15" si="14">LOG(D15/D$3, 2)*D$24</f>
-        <v>0</v>
+        <v>0.2240402742179301</v>
       </c>
       <c r="W15">
         <f t="shared" si="14"/>
@@ -6035,176 +6033,164 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="1">
-        <v>0.5</v>
+        <v>0.69199999999999995</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" ref="E16:E22" si="18">1/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>2.5669999999999998E-2</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" ref="F16:P22" si="19">1/24</f>
-        <v>4.1666666666666664E-2</v>
+        <v>2.5669999999999998E-2</v>
       </c>
       <c r="G16" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.5669999999999998E-2</v>
       </c>
       <c r="H16" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.5669999999999998E-2</v>
       </c>
       <c r="I16" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.5669999999999998E-2</v>
       </c>
       <c r="J16" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.5669999999999998E-2</v>
       </c>
       <c r="K16" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.5669999999999998E-2</v>
       </c>
       <c r="L16" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.5669999999999998E-2</v>
       </c>
       <c r="M16" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.5669999999999998E-2</v>
       </c>
       <c r="N16" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.5669999999999998E-2</v>
       </c>
       <c r="O16" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.5669999999999998E-2</v>
       </c>
       <c r="P16" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>2.5669999999999998E-2</v>
       </c>
       <c r="R16" s="3">
         <f t="shared" si="13"/>
-        <v>0.99999999999999956</v>
+        <v>1.0000399999999996</v>
       </c>
       <c r="T16" s="11">
-        <f t="shared" ref="T16:T22" si="20">SUM(V16:AH16)</f>
-        <v>0</v>
+        <f t="shared" ref="T16:T22" si="18">SUM(V16:AH16)</f>
+        <v>0.46884394297463744</v>
       </c>
       <c r="U16" s="13"/>
       <c r="V16">
-        <f t="shared" ref="V16:AH22" si="21">LOG(D16/D$3, 2)*D$24</f>
-        <v>0</v>
+        <f t="shared" ref="V16:AH22" si="19">LOG(D16/D$3, 2)*D$24</f>
+        <v>0.46884394297463744</v>
       </c>
       <c r="W16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Y16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AC16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AD16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AE16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AF16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AG16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AH16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AJ16">
-        <f t="shared" ref="AJ16:AJ22" si="22">D16*LOG((1/D16),2)</f>
-        <v>0.5</v>
+        <f t="shared" ref="AJ16:AJ22" si="20">D16*LOG((1/D16),2)</f>
+        <v>0.36755999146155083</v>
       </c>
       <c r="AK16">
-        <f t="shared" ref="AK16:AK22" si="23">E16*LOG((1/E16),2)</f>
-        <v>0.19104010419671485</v>
+        <f t="shared" ref="AK16:AK22" si="21">E16*LOG((1/E16),2)</f>
+        <v>0.13563445018542197</v>
       </c>
       <c r="AL16">
-        <f t="shared" ref="AL16:AL22" si="24">F16*LOG((1/F16),2)</f>
-        <v>0.19104010419671485</v>
+        <f t="shared" ref="AL16:AL22" si="22">F16*LOG((1/F16),2)</f>
+        <v>0.13563445018542197</v>
       </c>
       <c r="AM16">
-        <f t="shared" ref="AM16:AM22" si="25">G16*LOG((1/G16),2)</f>
-        <v>0.19104010419671485</v>
+        <f t="shared" ref="AM16:AM22" si="23">G16*LOG((1/G16),2)</f>
+        <v>0.13563445018542197</v>
       </c>
       <c r="AN16">
-        <f t="shared" ref="AN16:AN22" si="26">H16*LOG((1/H16),2)</f>
-        <v>0.19104010419671485</v>
+        <f t="shared" ref="AN16:AN22" si="24">H16*LOG((1/H16),2)</f>
+        <v>0.13563445018542197</v>
       </c>
       <c r="AO16">
-        <f t="shared" ref="AO16:AO22" si="27">I16*LOG((1/I16),2)</f>
-        <v>0.19104010419671485</v>
+        <f t="shared" ref="AO16:AO22" si="25">I16*LOG((1/I16),2)</f>
+        <v>0.13563445018542197</v>
       </c>
       <c r="AP16">
-        <f t="shared" ref="AP16:AP22" si="28">J16*LOG((1/J16),2)</f>
-        <v>0.19104010419671485</v>
+        <f t="shared" ref="AP16:AP22" si="26">J16*LOG((1/J16),2)</f>
+        <v>0.13563445018542197</v>
       </c>
       <c r="AQ16">
-        <f t="shared" ref="AQ16:AQ22" si="29">K16*LOG((1/K16),2)</f>
-        <v>0.19104010419671485</v>
+        <f t="shared" ref="AQ16:AQ22" si="27">K16*LOG((1/K16),2)</f>
+        <v>0.13563445018542197</v>
       </c>
       <c r="AR16">
-        <f t="shared" ref="AR16:AR22" si="30">L16*LOG((1/L16),2)</f>
-        <v>0.19104010419671485</v>
+        <f t="shared" ref="AR16:AR22" si="28">L16*LOG((1/L16),2)</f>
+        <v>0.13563445018542197</v>
       </c>
       <c r="AS16">
-        <f t="shared" ref="AS16:AS22" si="31">M16*LOG((1/M16),2)</f>
-        <v>0.19104010419671485</v>
+        <f t="shared" ref="AS16:AS22" si="29">M16*LOG((1/M16),2)</f>
+        <v>0.13563445018542197</v>
       </c>
       <c r="AT16">
-        <f t="shared" ref="AT16:AT22" si="32">N16*LOG((1/N16),2)</f>
-        <v>0.19104010419671485</v>
+        <f t="shared" ref="AT16:AT22" si="30">N16*LOG((1/N16),2)</f>
+        <v>0.13563445018542197</v>
       </c>
       <c r="AU16">
-        <f t="shared" ref="AU16:AU22" si="33">O16*LOG((1/O16),2)</f>
-        <v>0.19104010419671485</v>
+        <f t="shared" ref="AU16:AU22" si="31">O16*LOG((1/O16),2)</f>
+        <v>0.13563445018542197</v>
       </c>
       <c r="AV16">
-        <f t="shared" ref="AV16:AV22" si="34">P16*LOG((1/P16),2)</f>
-        <v>0.19104010419671485</v>
+        <f t="shared" ref="AV16:AV22" si="32">P16*LOG((1/P16),2)</f>
+        <v>0.13563445018542197</v>
       </c>
       <c r="AW16">
-        <f t="shared" ref="AW16:AW22" si="35">SUM(AJ16:AV16)</f>
-        <v>2.7924812503605789</v>
+        <f t="shared" ref="AW16:AW22" si="33">SUM(AJ16:AV16)</f>
+        <v>1.9951733936866138</v>
       </c>
       <c r="AY16" s="16">
-        <f t="shared" ref="AY16:AY22" si="36">($AW$3-AW16)/$AW$3</f>
-        <v>0</v>
+        <f t="shared" ref="AY16:AY22" si="34">($AW$3-AW16)/$AW$3</f>
+        <v>0.28551950226022565</v>
       </c>
     </row>
     <row r="17" spans="1:51" ht="18.75">
@@ -6216,176 +6202,164 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="1">
-        <v>0.5</v>
+        <v>0.76400000000000001</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="18"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.967E-2</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.967E-2</v>
       </c>
       <c r="G17" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.967E-2</v>
       </c>
       <c r="H17" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.967E-2</v>
       </c>
       <c r="I17" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.967E-2</v>
       </c>
       <c r="J17" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.967E-2</v>
       </c>
       <c r="K17" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.967E-2</v>
       </c>
       <c r="L17" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.967E-2</v>
       </c>
       <c r="M17" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.967E-2</v>
       </c>
       <c r="N17" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.967E-2</v>
       </c>
       <c r="O17" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.967E-2</v>
       </c>
       <c r="P17" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.967E-2</v>
       </c>
       <c r="R17" s="3">
         <f t="shared" si="13"/>
-        <v>0.99999999999999956</v>
+        <v>1.0000399999999996</v>
       </c>
       <c r="T17" s="11">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>0.6116445433736617</v>
       </c>
       <c r="U17" s="13"/>
       <c r="V17">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>0.6116445433736617</v>
       </c>
       <c r="W17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Y17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AC17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AD17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AE17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AF17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AG17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AH17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AJ17">
+        <f t="shared" si="20"/>
+        <v>0.29670356886252247</v>
+      </c>
+      <c r="AK17">
+        <f t="shared" si="21"/>
+        <v>0.11148679109655341</v>
+      </c>
+      <c r="AL17">
         <f t="shared" si="22"/>
-        <v>0.5</v>
-      </c>
-      <c r="AK17">
+        <v>0.11148679109655341</v>
+      </c>
+      <c r="AM17">
         <f t="shared" si="23"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AL17">
+        <v>0.11148679109655341</v>
+      </c>
+      <c r="AN17">
         <f t="shared" si="24"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AM17">
+        <v>0.11148679109655341</v>
+      </c>
+      <c r="AO17">
         <f t="shared" si="25"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AN17">
+        <v>0.11148679109655341</v>
+      </c>
+      <c r="AP17">
         <f t="shared" si="26"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AO17">
+        <v>0.11148679109655341</v>
+      </c>
+      <c r="AQ17">
         <f t="shared" si="27"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AP17">
+        <v>0.11148679109655341</v>
+      </c>
+      <c r="AR17">
         <f t="shared" si="28"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AQ17">
+        <v>0.11148679109655341</v>
+      </c>
+      <c r="AS17">
         <f t="shared" si="29"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AR17">
+        <v>0.11148679109655341</v>
+      </c>
+      <c r="AT17">
         <f t="shared" si="30"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AS17">
+        <v>0.11148679109655341</v>
+      </c>
+      <c r="AU17">
         <f t="shared" si="31"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AT17">
+        <v>0.11148679109655341</v>
+      </c>
+      <c r="AV17">
         <f t="shared" si="32"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AU17">
+        <v>0.11148679109655341</v>
+      </c>
+      <c r="AW17">
         <f t="shared" si="33"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AV17">
+        <v>1.6345450620211628</v>
+      </c>
+      <c r="AY17" s="16">
         <f t="shared" si="34"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AW17">
-        <f t="shared" si="35"/>
-        <v>2.7924812503605789</v>
-      </c>
-      <c r="AY17" s="16">
-        <f t="shared" si="36"/>
-        <v>0</v>
+        <v>0.41466211749493315</v>
       </c>
     </row>
     <row r="18" spans="1:51" ht="18.75">
@@ -6397,176 +6371,164 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="1">
-        <v>0.5</v>
+        <v>0.82399999999999995</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="18"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.4670000000000001E-2</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.4670000000000001E-2</v>
       </c>
       <c r="G18" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.4670000000000001E-2</v>
       </c>
       <c r="H18" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.4670000000000001E-2</v>
       </c>
       <c r="I18" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.4670000000000001E-2</v>
       </c>
       <c r="J18" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.4670000000000001E-2</v>
       </c>
       <c r="K18" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.4670000000000001E-2</v>
       </c>
       <c r="L18" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.4670000000000001E-2</v>
       </c>
       <c r="M18" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.4670000000000001E-2</v>
       </c>
       <c r="N18" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.4670000000000001E-2</v>
       </c>
       <c r="O18" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.4670000000000001E-2</v>
       </c>
       <c r="P18" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.4670000000000001E-2</v>
       </c>
       <c r="R18" s="3">
         <f t="shared" si="13"/>
-        <v>0.99999999999999956</v>
+        <v>1.0000399999999996</v>
       </c>
       <c r="T18" s="11">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>0.72071624252113131</v>
       </c>
       <c r="U18" s="13"/>
       <c r="V18">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>0.72071624252113131</v>
       </c>
       <c r="W18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Y18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AB18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AC18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AD18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AE18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AF18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AG18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AH18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AJ18">
+        <f t="shared" si="20"/>
+        <v>0.23012981616258787</v>
+      </c>
+      <c r="AK18">
+        <f t="shared" si="21"/>
+        <v>8.9354783966259399E-2</v>
+      </c>
+      <c r="AL18">
         <f t="shared" si="22"/>
-        <v>0.5</v>
-      </c>
-      <c r="AK18">
+        <v>8.9354783966259399E-2</v>
+      </c>
+      <c r="AM18">
         <f t="shared" si="23"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AL18">
+        <v>8.9354783966259399E-2</v>
+      </c>
+      <c r="AN18">
         <f t="shared" si="24"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AM18">
+        <v>8.9354783966259399E-2</v>
+      </c>
+      <c r="AO18">
         <f t="shared" si="25"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AN18">
+        <v>8.9354783966259399E-2</v>
+      </c>
+      <c r="AP18">
         <f t="shared" si="26"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AO18">
+        <v>8.9354783966259399E-2</v>
+      </c>
+      <c r="AQ18">
         <f t="shared" si="27"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AP18">
+        <v>8.9354783966259399E-2</v>
+      </c>
+      <c r="AR18">
         <f t="shared" si="28"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AQ18">
+        <v>8.9354783966259399E-2</v>
+      </c>
+      <c r="AS18">
         <f t="shared" si="29"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AR18">
+        <v>8.9354783966259399E-2</v>
+      </c>
+      <c r="AT18">
         <f t="shared" si="30"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AS18">
+        <v>8.9354783966259399E-2</v>
+      </c>
+      <c r="AU18">
         <f t="shared" si="31"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AT18">
+        <v>8.9354783966259399E-2</v>
+      </c>
+      <c r="AV18">
         <f t="shared" si="32"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AU18">
+        <v>8.9354783966259399E-2</v>
+      </c>
+      <c r="AW18">
         <f t="shared" si="33"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AV18">
+        <v>1.3023872237577006</v>
+      </c>
+      <c r="AY18" s="16">
         <f t="shared" si="34"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AW18">
-        <f t="shared" si="35"/>
-        <v>2.7924812503605789</v>
-      </c>
-      <c r="AY18" s="16">
-        <f t="shared" si="36"/>
-        <v>0</v>
+        <v>0.53360932196428179</v>
       </c>
     </row>
     <row r="19" spans="1:51" ht="18.75">
@@ -6578,176 +6540,164 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="1">
-        <v>0.5</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="18"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2670000000000001E-2</v>
       </c>
       <c r="F19" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2670000000000001E-2</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2670000000000001E-2</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2670000000000001E-2</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2670000000000001E-2</v>
       </c>
       <c r="J19" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2670000000000001E-2</v>
       </c>
       <c r="K19" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2670000000000001E-2</v>
       </c>
       <c r="L19" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2670000000000001E-2</v>
       </c>
       <c r="M19" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2670000000000001E-2</v>
       </c>
       <c r="N19" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2670000000000001E-2</v>
       </c>
       <c r="O19" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2670000000000001E-2</v>
       </c>
       <c r="P19" s="4">
-        <f t="shared" si="19"/>
-        <v>4.1666666666666664E-2</v>
+        <v>1.2670000000000001E-2</v>
       </c>
       <c r="R19" s="3">
         <f t="shared" si="13"/>
-        <v>0.99999999999999956</v>
+        <v>1.0000399999999996</v>
       </c>
       <c r="T19" s="11">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <f t="shared" si="18"/>
+        <v>0.76213616990111199</v>
       </c>
       <c r="U19" s="13"/>
       <c r="V19">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="19"/>
+        <v>0.76213616990111199</v>
       </c>
       <c r="W19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Y19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AB19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AC19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AD19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AE19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AF19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AG19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AH19">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AJ19">
+        <f t="shared" si="20"/>
+        <v>0.20170852792385699</v>
+      </c>
+      <c r="AK19">
+        <f t="shared" si="21"/>
+        <v>7.9851910559300354E-2</v>
+      </c>
+      <c r="AL19">
         <f t="shared" si="22"/>
-        <v>0.5</v>
-      </c>
-      <c r="AK19">
+        <v>7.9851910559300354E-2</v>
+      </c>
+      <c r="AM19">
         <f t="shared" si="23"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AL19">
+        <v>7.9851910559300354E-2</v>
+      </c>
+      <c r="AN19">
         <f t="shared" si="24"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AM19">
+        <v>7.9851910559300354E-2</v>
+      </c>
+      <c r="AO19">
         <f t="shared" si="25"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AN19">
+        <v>7.9851910559300354E-2</v>
+      </c>
+      <c r="AP19">
         <f t="shared" si="26"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AO19">
+        <v>7.9851910559300354E-2</v>
+      </c>
+      <c r="AQ19">
         <f t="shared" si="27"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AP19">
+        <v>7.9851910559300354E-2</v>
+      </c>
+      <c r="AR19">
         <f t="shared" si="28"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AQ19">
+        <v>7.9851910559300354E-2</v>
+      </c>
+      <c r="AS19">
         <f t="shared" si="29"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AR19">
+        <v>7.9851910559300354E-2</v>
+      </c>
+      <c r="AT19">
         <f t="shared" si="30"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AS19">
+        <v>7.9851910559300354E-2</v>
+      </c>
+      <c r="AU19">
         <f t="shared" si="31"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AT19">
+        <v>7.9851910559300354E-2</v>
+      </c>
+      <c r="AV19">
         <f t="shared" si="32"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AU19">
+        <v>7.9851910559300354E-2</v>
+      </c>
+      <c r="AW19">
         <f t="shared" si="33"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AV19">
+        <v>1.1599314546354609</v>
+      </c>
+      <c r="AY19" s="16">
         <f t="shared" si="34"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AW19">
-        <f t="shared" si="35"/>
-        <v>2.7924812503605789</v>
-      </c>
-      <c r="AY19" s="16">
-        <f t="shared" si="36"/>
-        <v>0</v>
+        <v>0.58462336873857801</v>
       </c>
     </row>
     <row r="20" spans="1:51" ht="18.75">
@@ -6762,51 +6712,51 @@
         <v>0.5</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="E16:E22" si="35">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="F16:P22" si="36">1/24</f>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I20" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J20" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K20" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L20" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M20" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N20" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O20" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P20" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R20" s="3">
@@ -6814,120 +6764,120 @@
         <v>0.99999999999999956</v>
       </c>
       <c r="T20" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U20" s="13"/>
       <c r="V20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AB20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AC20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AD20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AE20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AF20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AG20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AH20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AJ20">
+        <f t="shared" si="20"/>
+        <v>0.5</v>
+      </c>
+      <c r="AK20">
+        <f t="shared" si="21"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AL20">
         <f t="shared" si="22"/>
-        <v>0.5</v>
-      </c>
-      <c r="AK20">
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AM20">
         <f t="shared" si="23"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AL20">
+      <c r="AN20">
         <f t="shared" si="24"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AM20">
+      <c r="AO20">
         <f t="shared" si="25"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AN20">
+      <c r="AP20">
         <f t="shared" si="26"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AO20">
+      <c r="AQ20">
         <f t="shared" si="27"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AP20">
+      <c r="AR20">
         <f t="shared" si="28"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AQ20">
+      <c r="AS20">
         <f t="shared" si="29"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AR20">
+      <c r="AT20">
         <f t="shared" si="30"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AS20">
+      <c r="AU20">
         <f t="shared" si="31"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AT20">
+      <c r="AV20">
         <f t="shared" si="32"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AU20">
+      <c r="AW20">
         <f t="shared" si="33"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AV20">
+        <v>2.7924812503605789</v>
+      </c>
+      <c r="AY20" s="16">
         <f t="shared" si="34"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AW20">
-        <f t="shared" si="35"/>
-        <v>2.7924812503605789</v>
-      </c>
-      <c r="AY20" s="16">
-        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -6943,51 +6893,51 @@
         <v>0.5</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="35"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F21" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J21" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K21" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L21" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M21" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N21" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O21" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P21" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R21" s="3">
@@ -6995,120 +6945,120 @@
         <v>0.99999999999999956</v>
       </c>
       <c r="T21" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U21" s="13"/>
       <c r="V21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Z21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AB21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AC21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AD21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AE21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AF21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AG21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AH21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AJ21">
+        <f t="shared" si="20"/>
+        <v>0.5</v>
+      </c>
+      <c r="AK21">
+        <f t="shared" si="21"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AL21">
         <f t="shared" si="22"/>
-        <v>0.5</v>
-      </c>
-      <c r="AK21">
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AM21">
         <f t="shared" si="23"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AL21">
+      <c r="AN21">
         <f t="shared" si="24"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AM21">
+      <c r="AO21">
         <f t="shared" si="25"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AN21">
+      <c r="AP21">
         <f t="shared" si="26"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AO21">
+      <c r="AQ21">
         <f t="shared" si="27"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AP21">
+      <c r="AR21">
         <f t="shared" si="28"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AQ21">
+      <c r="AS21">
         <f t="shared" si="29"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AR21">
+      <c r="AT21">
         <f t="shared" si="30"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AS21">
+      <c r="AU21">
         <f t="shared" si="31"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AT21">
+      <c r="AV21">
         <f t="shared" si="32"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AU21">
+      <c r="AW21">
         <f t="shared" si="33"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AV21">
+        <v>2.7924812503605789</v>
+      </c>
+      <c r="AY21" s="16">
         <f t="shared" si="34"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AW21">
-        <f t="shared" si="35"/>
-        <v>2.7924812503605789</v>
-      </c>
-      <c r="AY21" s="16">
-        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -7124,51 +7074,51 @@
         <v>0.5</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="35"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="K22" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="L22" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="M22" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="N22" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="O22" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="P22" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="36"/>
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="R22" s="3">
@@ -7176,120 +7126,120 @@
         <v>0.99999999999999956</v>
       </c>
       <c r="T22" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U22" s="13"/>
       <c r="V22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="W22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="X22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AB22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AC22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AD22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AE22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AF22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AG22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AH22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="AJ22">
+        <f t="shared" si="20"/>
+        <v>0.5</v>
+      </c>
+      <c r="AK22">
+        <f t="shared" si="21"/>
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AL22">
         <f t="shared" si="22"/>
-        <v>0.5</v>
-      </c>
-      <c r="AK22">
+        <v>0.19104010419671485</v>
+      </c>
+      <c r="AM22">
         <f t="shared" si="23"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AL22">
+      <c r="AN22">
         <f t="shared" si="24"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AM22">
+      <c r="AO22">
         <f t="shared" si="25"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AN22">
+      <c r="AP22">
         <f t="shared" si="26"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AO22">
+      <c r="AQ22">
         <f t="shared" si="27"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AP22">
+      <c r="AR22">
         <f t="shared" si="28"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AQ22">
+      <c r="AS22">
         <f t="shared" si="29"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AR22">
+      <c r="AT22">
         <f t="shared" si="30"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AS22">
+      <c r="AU22">
         <f t="shared" si="31"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AT22">
+      <c r="AV22">
         <f t="shared" si="32"/>
         <v>0.19104010419671485</v>
       </c>
-      <c r="AU22">
+      <c r="AW22">
         <f t="shared" si="33"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AV22">
+        <v>2.7924812503605789</v>
+      </c>
+      <c r="AY22" s="16">
         <f t="shared" si="34"/>
-        <v>0.19104010419671485</v>
-      </c>
-      <c r="AW22">
-        <f t="shared" si="35"/>
-        <v>2.7924812503605789</v>
-      </c>
-      <c r="AY22" s="16">
-        <f t="shared" si="36"/>
         <v>0</v>
       </c>
     </row>
@@ -7304,7 +7254,7 @@
     </row>
     <row r="24" spans="1:51" ht="18.75">
       <c r="D24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
@@ -7344,11 +7294,11 @@
       </c>
       <c r="R24" s="3">
         <f>SUM(D24:P24)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T24" s="14">
         <f>AVERAGE(T15:T22)</f>
-        <v>0</v>
+        <v>0.34842264662355904</v>
       </c>
     </row>
     <row r="25" spans="1:51">

</xml_diff>